<commit_message>
change the xlsx filename
</commit_message>
<xml_diff>
--- a/lwf09.xlsx
+++ b/lwf09.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
     <sheet name="Reach Propertise" sheetId="1" r:id="rId2"/>
     <sheet name="Initial Concentration" sheetId="10" r:id="rId3"/>
     <sheet name="Loading" sheetId="3" r:id="rId4"/>
-    <sheet name="hidden tab" sheetId="11" state="hidden" r:id="rId5"/>
+    <sheet name="hidden tab" sheetId="11" r:id="rId5"/>
     <sheet name="LDC" sheetId="12" r:id="rId6"/>
     <sheet name="چاتا" sheetId="14" r:id="rId7"/>
     <sheet name="ماکیناو" sheetId="15" r:id="rId8"/>
@@ -25,7 +25,7 @@
     <definedName name="deltaX">Setting!$G$7:$G$15</definedName>
     <definedName name="Longitudinal_Disspersion_Coefficient">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -376,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1426,15 +1426,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1477,6 +1468,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2767,7 +2767,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2866,6 +2866,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2947,6 +2952,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3028,6 +3038,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3109,6 +3124,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -3190,6 +3210,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -3271,6 +3296,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -3358,6 +3388,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -3445,6 +3480,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -3532,6 +3572,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-1F35-48D0-949A-911C542FE41A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4663,13 +4708,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" style="76" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="73" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="67"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -4697,7 +4742,7 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="65" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="7"/>
@@ -4727,7 +4772,7 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="69">
+      <c r="B3" s="66">
         <f>DATE(1990,7,28)</f>
         <v>33082</v>
       </c>
@@ -4758,7 +4803,7 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="65" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7"/>
@@ -4788,7 +4833,7 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="65" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7"/>
@@ -4818,9 +4863,9 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="70" t="str">
+      <c r="B6" s="67" t="str">
         <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
-        <v>C:\Users\Mostafa Ramezani\Documents\MATLAB\</v>
+        <v>C:\Users\Mostafa\Dropbox\Science\watum\</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -4847,7 +4892,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="71"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -4875,7 +4920,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="67"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -4903,7 +4948,7 @@
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="72">
+      <c r="B9" s="69">
         <v>50</v>
       </c>
       <c r="C9" s="7"/>
@@ -4933,7 +4978,7 @@
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="72">
+      <c r="B10" s="69">
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
@@ -4963,7 +5008,7 @@
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="70" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="7"/>
@@ -4993,7 +5038,7 @@
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="72">
+      <c r="B12" s="69">
         <v>50</v>
       </c>
       <c r="C12" s="7"/>
@@ -5023,7 +5068,7 @@
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74">
+      <c r="B13" s="71">
         <v>0</v>
       </c>
       <c r="C13" s="7"/>
@@ -5053,7 +5098,7 @@
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="72">
+      <c r="B14" s="69">
         <v>0.5</v>
       </c>
       <c r="C14" s="7"/>
@@ -5081,7 +5126,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="71"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -5107,7 +5152,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="71"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -5133,7 +5178,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="71"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -5159,7 +5204,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="71"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -5185,7 +5230,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="71"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -5211,7 +5256,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="75"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -5237,7 +5282,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="71"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -5263,7 +5308,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="71"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -5289,7 +5334,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="B23" s="71"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -5315,7 +5360,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="71"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -5341,7 +5386,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="71"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -5367,7 +5412,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="71"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -5393,7 +5438,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="71"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -5419,7 +5464,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="71"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -5445,7 +5490,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="71"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -5471,7 +5516,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="71"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -5497,7 +5542,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="71"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -5523,7 +5568,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
-      <c r="B32" s="71"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -5549,7 +5594,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="71"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -5575,7 +5620,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="71"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -5601,7 +5646,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="71"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -5627,7 +5672,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
-      <c r="B36" s="71"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -5653,7 +5698,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="B37" s="71"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -5679,7 +5724,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="B38" s="71"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -5705,7 +5750,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="B39" s="71"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -5731,7 +5776,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="B40" s="71"/>
+      <c r="B40" s="68"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -5757,7 +5802,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
-      <c r="B41" s="71"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -5783,7 +5828,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
-      <c r="B42" s="71"/>
+      <c r="B42" s="68"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -5809,7 +5854,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
-      <c r="B43" s="71"/>
+      <c r="B43" s="68"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -5835,7 +5880,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
-      <c r="B44" s="71"/>
+      <c r="B44" s="68"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -5861,7 +5906,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
-      <c r="B45" s="71"/>
+      <c r="B45" s="68"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -5887,7 +5932,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
-      <c r="B46" s="71"/>
+      <c r="B46" s="68"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -5913,7 +5958,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
-      <c r="B47" s="71"/>
+      <c r="B47" s="68"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -5939,7 +5984,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
-      <c r="B48" s="71"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -5965,7 +6010,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
-      <c r="B49" s="71"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -5991,7 +6036,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
-      <c r="B50" s="71"/>
+      <c r="B50" s="68"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -6017,7 +6062,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
-      <c r="B51" s="71"/>
+      <c r="B51" s="68"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
@@ -6043,7 +6088,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
-      <c r="B52" s="71"/>
+      <c r="B52" s="68"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
@@ -6069,7 +6114,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
-      <c r="B53" s="71"/>
+      <c r="B53" s="68"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -6095,7 +6140,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
-      <c r="B54" s="71"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -6121,7 +6166,7 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
-      <c r="B55" s="71"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -6147,7 +6192,7 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
-      <c r="B56" s="71"/>
+      <c r="B56" s="68"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
@@ -6173,7 +6218,7 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
-      <c r="B57" s="71"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -6199,7 +6244,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
-      <c r="B58" s="71"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -6225,7 +6270,7 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="B59" s="71"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
@@ -6251,7 +6296,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
-      <c r="B60" s="71"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -6277,7 +6322,7 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
-      <c r="B61" s="71"/>
+      <c r="B61" s="68"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -6303,7 +6348,7 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
-      <c r="B62" s="71"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -6329,7 +6374,7 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
-      <c r="B63" s="71"/>
+      <c r="B63" s="68"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -7527,41 +7572,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="75" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7595,80 +7640,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="79" t="s">
+      <c r="L1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="76" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="80">
+      <c r="A2" s="77">
         <v>55</v>
       </c>
       <c r="B2" s="15">
         <v>1800</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="78">
         <v>0</v>
       </c>
-      <c r="D2" s="80">
+      <c r="D2" s="77">
         <v>15</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
       <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I4" s="27"/>
@@ -7684,11 +7729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
@@ -7849,7 +7897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8763,15 +8811,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="60"/>
-      <c r="G28" s="64" t="s">
+      <c r="G28" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="66"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="81"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="61" t="s">

</xml_diff>